<commit_message>
removed old, wrong path loss exponent estimates
</commit_message>
<xml_diff>
--- a/ExperimentalResults/rangingDataTwoFloors.xlsx
+++ b/ExperimentalResults/rangingDataTwoFloors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tori\Documents\Master-Thesis\indoor-positioning-for-bim\ExperimentalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0E2620-A34A-400E-B6D2-E830F9BE4E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243C4DBA-C51E-4FFD-BB33-33A20010755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Export" sheetId="1" r:id="rId1"/>
@@ -161,18 +161,6 @@
     <t>n estimates:</t>
   </si>
   <si>
-    <t>New average</t>
-  </si>
-  <si>
-    <t>new median</t>
-  </si>
-  <si>
-    <t>new min</t>
-  </si>
-  <si>
-    <t>new max</t>
-  </si>
-  <si>
     <t>RSS Distance</t>
   </si>
   <si>
@@ -204,6 +192,18 @@
   </si>
   <si>
     <t>Under 10000</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -7956,7 +7956,7 @@
         <v>1</v>
       </c>
       <c r="S7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T7" s="45">
         <f>COUNTIFS(L2:L231, "&gt;0",L2:L231,"&lt;1000")/COUNTIF(L2:L231,"&gt;0")</f>
@@ -8023,7 +8023,7 @@
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="T8" s="45">
         <f>COUNTIFS(L2:L231, "&gt;0",L2:L231,"&lt;2000")/COUNTIF(L2:L231,"&gt;0")</f>
@@ -8090,7 +8090,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T9" s="45">
         <f>COUNTIFS(L2:L231, "&gt;0",L2:L231,"&lt;3000")/COUNTIF(L2:L231,"&gt;0")</f>
@@ -8150,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="T10" s="45">
         <f>COUNTIFS(L2:L231, "&gt;0",L2:L231,"&lt;5000")/COUNTIF(L2:L231,"&gt;0")</f>
@@ -8210,7 +8210,7 @@
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="T11" s="45">
         <f>COUNTIFS(L2:L231, "&gt;0",L2:L231,"&lt;10000")/COUNTIF(L2:L231,"&gt;0")</f>
@@ -19892,8 +19892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662030DB-CAED-45E0-8832-8AB7268EC91D}">
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19951,7 +19951,7 @@
         <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
         <v>29</v>
@@ -19978,7 +19978,7 @@
         <v>33</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -20045,7 +20045,7 @@
         <v>2.2412012615916064</v>
       </c>
       <c r="U2">
-        <f>ABS(K2-J2)</f>
+        <f t="shared" ref="U2:U7" si="2">ABS(K2-J2)</f>
         <v>4778.7654393219054</v>
       </c>
     </row>
@@ -20082,7 +20082,7 @@
         <v>17897</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K7" si="2">1000*10^(($R3-$P3)/(10*$D$62))</f>
+        <f t="shared" ref="K3:K7" si="3">1000*10^(($R3-$P3)/(10*$D$62))</f>
         <v>6770.8149419470628</v>
       </c>
       <c r="L3">
@@ -20109,24 +20109,24 @@
         <v>-42</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S52" si="3">-(P3-R3)/(10*LOG10(J3/1000))</f>
+        <f t="shared" ref="S3:S52" si="4">-(P3-R3)/(10*LOG10(J3/1000))</f>
         <v>1.5964491929096054</v>
       </c>
       <c r="U3">
-        <f>ABS(K3-J3)</f>
+        <f t="shared" si="2"/>
         <v>11126.185058052937</v>
       </c>
       <c r="X3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Y3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Z3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AA3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -20162,7 +20162,7 @@
         <v>23526</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37863.24167439231</v>
       </c>
       <c r="L4">
@@ -20189,11 +20189,11 @@
         <v>-42</v>
       </c>
       <c r="S4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7705918737155955</v>
       </c>
       <c r="U4">
-        <f>ABS(K4-J4)</f>
+        <f t="shared" si="2"/>
         <v>14337.24167439231</v>
       </c>
       <c r="X4">
@@ -20246,7 +20246,7 @@
         <v>22199</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25827.930238510504</v>
       </c>
       <c r="L5">
@@ -20273,11 +20273,11 @@
         <v>-42</v>
       </c>
       <c r="S5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5253774226555494</v>
       </c>
       <c r="U5">
-        <f>ABS(K5-J5)</f>
+        <f t="shared" si="2"/>
         <v>3628.9302385105038</v>
       </c>
     </row>
@@ -20314,7 +20314,7 @@
         <v>8046</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5592.1247293023907</v>
       </c>
       <c r="L6">
@@ -20341,27 +20341,27 @@
         <v>-42</v>
       </c>
       <c r="S6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9876763443069374</v>
       </c>
       <c r="U6">
-        <f>ABS(K6-J6)</f>
+        <f t="shared" si="2"/>
         <v>2453.8752706976093</v>
       </c>
       <c r="X6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Y6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Z6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" t="s">
         <v>45</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -20397,7 +20397,7 @@
         <v>29752</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108410.24169482473</v>
       </c>
       <c r="L7">
@@ -20424,11 +20424,11 @@
         <v>-42</v>
       </c>
       <c r="S7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3253791951668688</v>
       </c>
       <c r="U7">
-        <f>ABS(K7-J7)</f>
+        <f t="shared" si="2"/>
         <v>78658.241694824726</v>
       </c>
       <c r="X7" s="45">
@@ -20485,14 +20485,14 @@
         <v>29840</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K14" si="4">1000*10^(($R9-$P9)/(10*$D$62))</f>
+        <f t="shared" ref="K9:K14" si="5">1000*10^(($R9-$P9)/(10*$D$62))</f>
         <v>89537.758554798493</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M14" si="5">ROUND(IF(O9,L9-J9,0),1)</f>
+        <f t="shared" ref="M9:M14" si="6">ROUND(IF(O9,L9-J9,0),1)</f>
         <v>0</v>
       </c>
       <c r="N9">
@@ -20505,18 +20505,18 @@
         <v>-87</v>
       </c>
       <c r="Q9" t="b">
-        <f t="shared" ref="Q9:Q14" si="6">ABS($M9)-N9&lt;0</f>
+        <f t="shared" ref="Q9:Q14" si="7">ABS($M9)-N9&lt;0</f>
         <v>0</v>
       </c>
       <c r="R9">
         <v>-40</v>
       </c>
       <c r="S9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.1868753487490853</v>
       </c>
       <c r="U9">
-        <f>ABS(K9-J9)</f>
+        <f t="shared" ref="U9:U14" si="8">ABS(K9-J9)</f>
         <v>59697.758554798493</v>
       </c>
     </row>
@@ -20553,14 +20553,14 @@
         <v>21188</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55506.773359479026</v>
       </c>
       <c r="L10">
         <v>26812</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5624</v>
       </c>
       <c r="N10">
@@ -20573,18 +20573,18 @@
         <v>-82</v>
       </c>
       <c r="Q10" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R10">
         <v>-40</v>
       </c>
       <c r="S10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.1672059311092493</v>
       </c>
       <c r="U10">
-        <f>ABS(K10-J10)</f>
+        <f t="shared" si="8"/>
         <v>34318.773359479026</v>
       </c>
     </row>
@@ -20621,14 +20621,14 @@
         <v>17234</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16011.402264621549</v>
       </c>
       <c r="L11">
         <v>17250</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="N11">
@@ -20641,18 +20641,18 @@
         <v>-69</v>
       </c>
       <c r="Q11" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R11">
         <v>-40</v>
       </c>
       <c r="S11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.345545640408615</v>
       </c>
       <c r="U11">
-        <f>ABS(K11-J11)</f>
+        <f t="shared" si="8"/>
         <v>1222.597735378451</v>
       </c>
     </row>
@@ -20689,14 +20689,14 @@
         <v>7829</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144433.00739347163</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N12">
@@ -20709,18 +20709,18 @@
         <v>-92</v>
       </c>
       <c r="Q12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R12">
         <v>-40</v>
       </c>
       <c r="S12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8184663578546232</v>
       </c>
       <c r="U12">
-        <f>ABS(K12-J12)</f>
+        <f t="shared" si="8"/>
         <v>136604.00739347163</v>
       </c>
     </row>
@@ -20757,14 +20757,14 @@
         <v>32064</v>
       </c>
       <c r="K13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108410.24169482473</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N13">
@@ -20777,18 +20777,18 @@
         <v>-89</v>
       </c>
       <c r="Q13" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R13">
         <v>-40</v>
       </c>
       <c r="S13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2536138190702242</v>
       </c>
       <c r="U13">
-        <f>ABS(K13-J13)</f>
+        <f t="shared" si="8"/>
         <v>76346.241694824726</v>
       </c>
     </row>
@@ -20825,14 +20825,14 @@
         <v>11586</v>
       </c>
       <c r="K14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17618.195138757146</v>
       </c>
       <c r="L14">
         <v>14062</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2476</v>
       </c>
       <c r="N14">
@@ -20845,18 +20845,18 @@
         <v>-70</v>
       </c>
       <c r="Q14" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R14">
         <v>-40</v>
       </c>
       <c r="S14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8197250409606198</v>
       </c>
       <c r="U14">
-        <f>ABS(K14-J14)</f>
+        <f t="shared" si="8"/>
         <v>6032.1951387571462</v>
       </c>
     </row>
@@ -20893,14 +20893,14 @@
         <v>11728</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K24" si="7">1000*10^(($R16-$P16)/(10*$D$62))</f>
+        <f t="shared" ref="K16:K24" si="9">1000*10^(($R16-$P16)/(10*$D$62))</f>
         <v>9925.8825663574626</v>
       </c>
       <c r="L16">
         <v>12750</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M24" si="8">ROUND(IF(O16,L16-J16,0),1)</f>
+        <f t="shared" ref="M16:M24" si="10">ROUND(IF(O16,L16-J16,0),1)</f>
         <v>1022</v>
       </c>
       <c r="N16">
@@ -20913,18 +20913,18 @@
         <v>-65</v>
       </c>
       <c r="Q16" t="b">
-        <f t="shared" ref="Q16:Q24" si="9">ABS($M16)-N16&lt;0</f>
+        <f t="shared" ref="Q16:Q24" si="11">ABS($M16)-N16&lt;0</f>
         <v>0</v>
       </c>
       <c r="R16">
         <v>-41</v>
       </c>
       <c r="S16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2446186167274864</v>
       </c>
       <c r="U16">
-        <f>ABS(K16-J16)</f>
+        <f t="shared" ref="U16:U24" si="12">ABS(K16-J16)</f>
         <v>1802.1174336425374</v>
       </c>
     </row>
@@ -20961,14 +20961,14 @@
         <v>5721</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6153.3114397365198</v>
       </c>
       <c r="L17">
         <v>6562</v>
       </c>
       <c r="M17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>841</v>
       </c>
       <c r="N17">
@@ -20981,18 +20981,18 @@
         <v>-60</v>
       </c>
       <c r="Q17" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R17">
         <v>-41</v>
       </c>
       <c r="S17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5083437157038917</v>
       </c>
       <c r="U17">
-        <f>ABS(K17-J17)</f>
+        <f t="shared" si="12"/>
         <v>432.31143973651979</v>
       </c>
     </row>
@@ -21029,14 +21029,14 @@
         <v>5253</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4618.6255651941628</v>
       </c>
       <c r="L18">
         <v>5687</v>
       </c>
       <c r="M18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>434</v>
       </c>
       <c r="N18">
@@ -21049,18 +21049,18 @@
         <v>-57</v>
       </c>
       <c r="Q18" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R18">
         <v>-41</v>
       </c>
       <c r="S18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2209655234195589</v>
       </c>
       <c r="U18">
-        <f>ABS(K18-J18)</f>
+        <f t="shared" si="12"/>
         <v>634.37443480583715</v>
       </c>
     </row>
@@ -21097,14 +21097,14 @@
         <v>5732</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>108410.24169482473</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N19">
@@ -21117,18 +21117,18 @@
         <v>-90</v>
       </c>
       <c r="Q19" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R19">
         <v>-41</v>
       </c>
       <c r="S19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4617698208017558</v>
       </c>
       <c r="U19">
-        <f>ABS(K19-J19)</f>
+        <f t="shared" si="12"/>
         <v>102678.24169482473</v>
       </c>
     </row>
@@ -21165,14 +21165,14 @@
         <v>6783</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67206.313992305004</v>
       </c>
       <c r="L20">
         <v>19187</v>
       </c>
       <c r="M20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12404</v>
       </c>
       <c r="N20">
@@ -21185,18 +21185,18 @@
         <v>-85</v>
       </c>
       <c r="Q20" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R20">
         <v>-41</v>
       </c>
       <c r="S20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.2921392122380331</v>
       </c>
       <c r="U20">
-        <f>ABS(K20-J20)</f>
+        <f t="shared" si="12"/>
         <v>60423.313992305004</v>
       </c>
     </row>
@@ -21233,14 +21233,14 @@
         <v>6273</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>119289.53889563594</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N21">
@@ -21253,18 +21253,18 @@
         <v>-91</v>
       </c>
       <c r="Q21" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R21">
         <v>-41</v>
       </c>
       <c r="S21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.2697867609670874</v>
       </c>
       <c r="U21">
-        <f>ABS(K21-J21)</f>
+        <f t="shared" si="12"/>
         <v>113016.53889563594</v>
       </c>
     </row>
@@ -21301,14 +21301,14 @@
         <v>36315</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>41662.933038621799</v>
       </c>
       <c r="L22">
         <v>37187</v>
       </c>
       <c r="M22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>872</v>
       </c>
       <c r="N22">
@@ -21321,18 +21321,18 @@
         <v>-80</v>
       </c>
       <c r="Q22" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R22">
         <v>-41</v>
       </c>
       <c r="S22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4998621093729141</v>
       </c>
       <c r="U22">
-        <f>ABS(K22-J22)</f>
+        <f t="shared" si="12"/>
         <v>5347.9330386217989</v>
       </c>
     </row>
@@ -21369,14 +21369,14 @@
         <v>20830</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25827.930238510504</v>
       </c>
       <c r="L23">
         <v>26687</v>
       </c>
       <c r="M23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5857</v>
       </c>
       <c r="N23">
@@ -21389,18 +21389,18 @@
         <v>-75</v>
       </c>
       <c r="Q23" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R23">
         <v>-41</v>
       </c>
       <c r="S23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5783177868238267</v>
       </c>
       <c r="U23">
-        <f>ABS(K23-J23)</f>
+        <f t="shared" si="12"/>
         <v>4997.9302385105038</v>
       </c>
     </row>
@@ -21437,14 +21437,14 @@
         <v>10944</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7450.2867971292908</v>
       </c>
       <c r="L24">
         <v>11062</v>
       </c>
       <c r="M24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="N24">
@@ -21457,18 +21457,18 @@
         <v>-62</v>
       </c>
       <c r="Q24" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R24">
         <v>-41</v>
       </c>
       <c r="S24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0208317258002677</v>
       </c>
       <c r="U24">
-        <f>ABS(K24-J24)</f>
+        <f t="shared" si="12"/>
         <v>3493.7132028707092</v>
       </c>
     </row>
@@ -21505,14 +21505,14 @@
         <v>7582</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26:K37" si="10">1000*10^(($R26-$P26)/(10*$D$62))</f>
+        <f t="shared" ref="K26:K37" si="13">1000*10^(($R26-$P26)/(10*$D$62))</f>
         <v>2364.7673731896739</v>
       </c>
       <c r="L26">
         <v>7000</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:M37" si="11">ROUND(IF(O26,L26-J26,0),1)</f>
+        <f t="shared" ref="M26:M37" si="14">ROUND(IF(O26,L26-J26,0),1)</f>
         <v>-582</v>
       </c>
       <c r="N26">
@@ -21525,18 +21525,18 @@
         <v>-49</v>
       </c>
       <c r="Q26" t="b">
-        <f t="shared" ref="Q26:Q37" si="12">ABS($M26)-N26&lt;0</f>
+        <f t="shared" ref="Q26:Q37" si="15">ABS($M26)-N26&lt;0</f>
         <v>1</v>
       </c>
       <c r="R26">
         <v>-40</v>
       </c>
       <c r="S26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0229786231197699</v>
       </c>
       <c r="U26">
-        <f>ABS(K26-J26)</f>
+        <f t="shared" ref="U26:U37" si="16">ABS(K26-J26)</f>
         <v>5217.2326268103261</v>
       </c>
     </row>
@@ -21573,14 +21573,14 @@
         <v>13139</v>
       </c>
       <c r="K27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>119289.53889563594</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N27">
@@ -21593,18 +21593,18 @@
         <v>-90</v>
       </c>
       <c r="Q27" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R27">
         <v>-40</v>
       </c>
       <c r="S27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4700236576170633</v>
       </c>
       <c r="U27">
-        <f>ABS(K27-J27)</f>
+        <f t="shared" si="16"/>
         <v>106150.53889563594</v>
       </c>
     </row>
@@ -21641,14 +21641,14 @@
         <v>7943</v>
       </c>
       <c r="K28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>108410.24169482473</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N28">
@@ -21661,18 +21661,18 @@
         <v>-89</v>
       </c>
       <c r="Q28" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R28">
         <v>-40</v>
       </c>
       <c r="S28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.4445378330932082</v>
       </c>
       <c r="U28">
-        <f>ABS(K28-J28)</f>
+        <f t="shared" si="16"/>
         <v>100467.24169482473</v>
       </c>
     </row>
@@ -21709,14 +21709,14 @@
         <v>6541</v>
       </c>
       <c r="K29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>45843.934978093617</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N29">
@@ -21729,18 +21729,18 @@
         <v>-80</v>
       </c>
       <c r="Q29" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R29">
         <v>-40</v>
       </c>
       <c r="S29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9040994216128784</v>
       </c>
       <c r="U29">
-        <f>ABS(K29-J29)</f>
+        <f t="shared" si="16"/>
         <v>39302.934978093617</v>
       </c>
     </row>
@@ -21777,14 +21777,14 @@
         <v>3850</v>
       </c>
       <c r="K30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4618.6255651941628</v>
       </c>
       <c r="L30">
         <v>4937</v>
       </c>
       <c r="M30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1087</v>
       </c>
       <c r="N30">
@@ -21797,18 +21797,18 @@
         <v>-56</v>
       </c>
       <c r="Q30" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R30">
         <v>-40</v>
       </c>
       <c r="S30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.732890387615261</v>
       </c>
       <c r="U30">
-        <f>ABS(K30-J30)</f>
+        <f t="shared" si="16"/>
         <v>768.62556519416285</v>
       </c>
     </row>
@@ -21845,14 +21845,14 @@
         <v>7211</v>
       </c>
       <c r="K31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4618.6255651941628</v>
       </c>
       <c r="L31">
         <v>7750</v>
       </c>
       <c r="M31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>539</v>
       </c>
       <c r="N31">
@@ -21865,18 +21865,18 @@
         <v>-56</v>
       </c>
       <c r="Q31" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="R31">
         <v>-40</v>
       </c>
       <c r="S31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8648116549306384</v>
       </c>
       <c r="U31">
-        <f>ABS(K31-J31)</f>
+        <f t="shared" si="16"/>
         <v>2592.3744348058372</v>
       </c>
     </row>
@@ -21913,14 +21913,14 @@
         <v>6533</v>
       </c>
       <c r="K32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3814.5969813027041</v>
       </c>
       <c r="L32">
         <v>6562</v>
       </c>
       <c r="M32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="N32">
@@ -21933,18 +21933,18 @@
         <v>-54</v>
       </c>
       <c r="Q32" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="R32">
         <v>-40</v>
       </c>
       <c r="S32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7175539919955294</v>
       </c>
       <c r="U32">
-        <f>ABS(K32-J32)</f>
+        <f t="shared" si="16"/>
         <v>2718.4030186972959</v>
       </c>
     </row>
@@ -21981,14 +21981,14 @@
         <v>13173</v>
       </c>
       <c r="K33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>19386.234560678095</v>
       </c>
       <c r="L33">
         <v>17812</v>
       </c>
       <c r="M33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>4639</v>
       </c>
       <c r="N33">
@@ -22001,18 +22001,18 @@
         <v>-71</v>
       </c>
       <c r="Q33" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R33">
         <v>-40</v>
       </c>
       <c r="S33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7686365837063183</v>
       </c>
       <c r="U33">
-        <f>ABS(K33-J33)</f>
+        <f t="shared" si="16"/>
         <v>6213.2345606780946</v>
       </c>
     </row>
@@ -22049,14 +22049,14 @@
         <v>17846</v>
       </c>
       <c r="K34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>13224.07410666143</v>
       </c>
       <c r="L34">
         <v>17687</v>
       </c>
       <c r="M34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-159</v>
       </c>
       <c r="N34">
@@ -22069,18 +22069,18 @@
         <v>-67</v>
       </c>
       <c r="Q34" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="R34">
         <v>-40</v>
       </c>
       <c r="S34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1573406226563305</v>
       </c>
       <c r="U34">
-        <f>ABS(K34-J34)</f>
+        <f t="shared" si="16"/>
         <v>4621.9258933385699</v>
       </c>
     </row>
@@ -22117,14 +22117,14 @@
         <v>36821</v>
       </c>
       <c r="K35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>37863.24167439231</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N35">
@@ -22137,18 +22137,18 @@
         <v>-78</v>
       </c>
       <c r="Q35" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R35">
         <v>-40</v>
       </c>
       <c r="S35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4264164018886252</v>
       </c>
       <c r="U35">
-        <f>ABS(K35-J35)</f>
+        <f t="shared" si="16"/>
         <v>1042.2416743923095</v>
       </c>
     </row>
@@ -22185,14 +22185,14 @@
         <v>22289</v>
       </c>
       <c r="K36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>131260.60663152987</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N36">
@@ -22205,18 +22205,18 @@
         <v>-91</v>
       </c>
       <c r="Q36" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R36">
         <v>-40</v>
       </c>
       <c r="S36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7831285669587271</v>
       </c>
       <c r="U36">
-        <f>ABS(K36-J36)</f>
+        <f t="shared" si="16"/>
         <v>108971.60663152987</v>
       </c>
     </row>
@@ -22253,14 +22253,14 @@
         <v>10645</v>
       </c>
       <c r="K37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>119289.53889563594</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N37">
@@ -22273,18 +22273,18 @@
         <v>-90</v>
       </c>
       <c r="Q37" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R37">
         <v>-40</v>
       </c>
       <c r="S37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8678587337762025</v>
       </c>
       <c r="U37">
-        <f>ABS(K37-J37)</f>
+        <f t="shared" si="16"/>
         <v>108644.53889563594</v>
       </c>
     </row>
@@ -22321,14 +22321,14 @@
         <v>41747</v>
       </c>
       <c r="K39">
-        <f t="shared" ref="K39:K44" si="13">1000*10^(($R39-$P39)/(10*$D$62))</f>
+        <f t="shared" ref="K39:K44" si="17">1000*10^(($R39-$P39)/(10*$D$62))</f>
         <v>108410.24169482473</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39:M44" si="14">ROUND(IF(O39,L39-J39,0),1)</f>
+        <f t="shared" ref="M39:M44" si="18">ROUND(IF(O39,L39-J39,0),1)</f>
         <v>0</v>
       </c>
       <c r="N39">
@@ -22341,18 +22341,18 @@
         <v>-90</v>
       </c>
       <c r="Q39" t="b">
-        <f t="shared" ref="Q39:Q44" si="15">ABS($M39)-N39&lt;0</f>
+        <f t="shared" ref="Q39:Q44" si="19">ABS($M39)-N39&lt;0</f>
         <v>0</v>
       </c>
       <c r="R39">
         <v>-41</v>
       </c>
       <c r="S39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0235243673741721</v>
       </c>
       <c r="U39">
-        <f>ABS(K39-J39)</f>
+        <f t="shared" ref="U39:U44" si="20">ABS(K39-J39)</f>
         <v>66663.241694824726</v>
       </c>
       <c r="AB39">
@@ -22392,14 +22392,14 @@
         <v>25843</v>
       </c>
       <c r="K40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>34410.085069249879</v>
       </c>
       <c r="L40">
         <v>26500</v>
       </c>
       <c r="M40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>657</v>
       </c>
       <c r="N40">
@@ -22412,18 +22412,18 @@
         <v>-78</v>
       </c>
       <c r="Q40" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="R40">
         <v>-41</v>
       </c>
       <c r="S40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6197603483834668</v>
       </c>
       <c r="U40">
-        <f>ABS(K40-J40)</f>
+        <f t="shared" si="20"/>
         <v>8567.0850692498789</v>
       </c>
     </row>
@@ -22460,14 +22460,14 @@
         <v>14570</v>
       </c>
       <c r="K41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>119289.53889563594</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N41">
@@ -22480,18 +22480,18 @@
         <v>-91</v>
       </c>
       <c r="Q41" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R41">
         <v>-41</v>
       </c>
       <c r="S41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2975279994851716</v>
       </c>
       <c r="U41">
-        <f>ABS(K41-J41)</f>
+        <f t="shared" si="20"/>
         <v>104719.53889563594</v>
       </c>
     </row>
@@ -22528,14 +22528,14 @@
         <v>5379</v>
       </c>
       <c r="K42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>73950.671833988818</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N42">
@@ -22548,18 +22548,18 @@
         <v>-86</v>
       </c>
       <c r="Q42" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R42">
         <v>-41</v>
       </c>
       <c r="S42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.1584651561435129</v>
       </c>
       <c r="U42">
-        <f>ABS(K42-J42)</f>
+        <f t="shared" si="20"/>
         <v>68571.671833988818</v>
       </c>
     </row>
@@ -22596,14 +22596,14 @@
         <v>5388</v>
       </c>
       <c r="K43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2364.7673731896739</v>
       </c>
       <c r="L43">
         <v>4937</v>
       </c>
       <c r="M43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-451</v>
       </c>
       <c r="N43">
@@ -22616,18 +22616,18 @@
         <v>-50</v>
       </c>
       <c r="Q43" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="R43">
         <v>-41</v>
       </c>
       <c r="S43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2304704060024878</v>
       </c>
       <c r="U43">
-        <f>ABS(K43-J43)</f>
+        <f t="shared" si="20"/>
         <v>3023.2326268103261</v>
       </c>
     </row>
@@ -22664,14 +22664,14 @@
         <v>10729</v>
       </c>
       <c r="K44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>12018.028432046232</v>
       </c>
       <c r="L44">
         <v>12437</v>
       </c>
       <c r="M44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1708</v>
       </c>
       <c r="N44">
@@ -22684,18 +22684,18 @@
         <v>-67</v>
       </c>
       <c r="Q44" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R44">
         <v>-41</v>
       </c>
       <c r="S44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5229020183749289</v>
       </c>
       <c r="U44">
-        <f>ABS(K44-J44)</f>
+        <f t="shared" si="20"/>
         <v>1289.0284320462324</v>
       </c>
     </row>
@@ -22732,14 +22732,14 @@
         <v>30537</v>
       </c>
       <c r="K46">
-        <f t="shared" ref="K46:K52" si="16">1000*10^(($R46-$P46)/(10*$D$62))</f>
+        <f t="shared" ref="K46:K52" si="21">1000*10^(($R46-$P46)/(10*$D$62))</f>
         <v>81371.846480443273</v>
       </c>
       <c r="L46">
         <v>28937</v>
       </c>
       <c r="M46">
-        <f t="shared" ref="M46:M52" si="17">ROUND(IF(O46,L46-J46,0),1)</f>
+        <f t="shared" ref="M46:M52" si="22">ROUND(IF(O46,L46-J46,0),1)</f>
         <v>-1600</v>
       </c>
       <c r="N46">
@@ -22752,18 +22752,18 @@
         <v>-87</v>
       </c>
       <c r="Q46" t="b">
-        <f t="shared" ref="Q46:Q52" si="18">ABS($M46)-N46&lt;0</f>
+        <f t="shared" ref="Q46:Q52" si="23">ABS($M46)-N46&lt;0</f>
         <v>0</v>
       </c>
       <c r="R46">
         <v>-41</v>
       </c>
       <c r="S46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0980053262634346</v>
       </c>
       <c r="U46">
-        <f>ABS(K46-J46)</f>
+        <f t="shared" ref="U46:U52" si="24">ABS(K46-J46)</f>
         <v>50834.846480443273</v>
       </c>
     </row>
@@ -22800,14 +22800,14 @@
         <v>36502</v>
       </c>
       <c r="K47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>144433.00739347163</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N47">
@@ -22820,18 +22820,18 @@
         <v>-93</v>
       </c>
       <c r="Q47" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R47">
         <v>-41</v>
       </c>
       <c r="S47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3283905437341383</v>
       </c>
       <c r="U47">
-        <f>ABS(K47-J47)</f>
+        <f t="shared" si="24"/>
         <v>107931.00739347163</v>
       </c>
     </row>
@@ -22868,14 +22868,14 @@
         <v>30812</v>
       </c>
       <c r="K48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>23472.403243034314</v>
       </c>
       <c r="L48">
         <v>31187</v>
       </c>
       <c r="M48">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>375</v>
       </c>
       <c r="N48">
@@ -22888,18 +22888,18 @@
         <v>-74</v>
       </c>
       <c r="Q48" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="R48">
         <v>-41</v>
       </c>
       <c r="S48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2166695185333705</v>
       </c>
       <c r="U48">
-        <f>ABS(K48-J48)</f>
+        <f t="shared" si="24"/>
         <v>7339.5967569656859</v>
       </c>
     </row>
@@ -22936,14 +22936,14 @@
         <v>20338</v>
       </c>
       <c r="K49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>8197.9457178188841</v>
       </c>
       <c r="L49">
         <v>21437</v>
       </c>
       <c r="M49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>1099</v>
       </c>
       <c r="N49">
@@ -22956,18 +22956,18 @@
         <v>-63</v>
       </c>
       <c r="Q49" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R49">
         <v>-41</v>
       </c>
       <c r="S49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6815609102624784</v>
       </c>
       <c r="U49">
-        <f>ABS(K49-J49)</f>
+        <f t="shared" si="24"/>
         <v>12140.054282181116</v>
       </c>
     </row>
@@ -23004,14 +23004,14 @@
         <v>2141</v>
       </c>
       <c r="K50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1000</v>
       </c>
       <c r="L50">
         <v>1625</v>
       </c>
       <c r="M50">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-516</v>
       </c>
       <c r="N50">
@@ -23024,18 +23024,18 @@
         <v>-41</v>
       </c>
       <c r="Q50" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="R50">
         <v>-41</v>
       </c>
       <c r="S50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U50">
-        <f>ABS(K50-J50)</f>
+        <f t="shared" si="24"/>
         <v>1141</v>
       </c>
     </row>
@@ -23072,14 +23072,14 @@
         <v>5045</v>
       </c>
       <c r="K51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>9925.8825663574626</v>
       </c>
       <c r="L51">
         <v>6125</v>
       </c>
       <c r="M51">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>1080</v>
       </c>
       <c r="N51">
@@ -23092,18 +23092,18 @@
         <v>-65</v>
       </c>
       <c r="Q51" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R51">
         <v>-41</v>
       </c>
       <c r="S51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4146145789269693</v>
       </c>
       <c r="U51">
-        <f>ABS(K51-J51)</f>
+        <f t="shared" si="24"/>
         <v>4880.8825663574626</v>
       </c>
     </row>
@@ -23140,14 +23140,14 @@
         <v>17178</v>
       </c>
       <c r="K52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>131260.60663152987</v>
       </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N52">
@@ -23160,18 +23160,18 @@
         <v>-92</v>
       </c>
       <c r="Q52" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R52">
         <v>-41</v>
       </c>
       <c r="S52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1296462825052034</v>
       </c>
       <c r="U52">
-        <f>ABS(K52-J52)</f>
+        <f t="shared" si="24"/>
         <v>114082.60663152987</v>
       </c>
     </row>
@@ -23180,16 +23180,16 @@
         <v>34</v>
       </c>
       <c r="D61" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E61" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F61" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G61" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>